<commit_message>
Add nav bar to ALB
</commit_message>
<xml_diff>
--- a/screen_offsets.xlsx
+++ b/screen_offsets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>petrel</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>alb</t>
   </si>
 </sst>
 </file>
@@ -49,8 +52,16 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,9 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,15 +394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -400,13 +412,16 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <f>-0.156</f>
         <v>-0.156</v>
       </c>
@@ -414,8 +429,12 @@
         <f>0.39</f>
         <v>0.39</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f>0.0932</f>
+        <v>9.3200000000000005E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -423,16 +442,20 @@
         <f>D4-D$3</f>
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <f>-0.07</f>
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E4" s="1">
-        <f>$E$3+C4</f>
+        <f>E$3+$C4</f>
         <v>0.47599999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1">
+        <f>F$3+$C4</f>
+        <v>0.1792</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -440,16 +463,20 @@
         <f t="shared" ref="C5:C6" si="0">D5-D$3</f>
         <v>5.5999999999999994E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <f>-0.1</f>
         <v>-0.1</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E6" si="1">$E$3+C5</f>
+        <f t="shared" ref="E5:F6" si="1">E$3+$C5</f>
         <v>0.44600000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1492</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -457,7 +484,7 @@
         <f t="shared" si="0"/>
         <v>-0.23200000000000001</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <f>-0.388</f>
         <v>-0.38800000000000001</v>
       </c>
@@ -465,34 +492,42 @@
         <f t="shared" si="1"/>
         <v>0.158</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.13880000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>2.7130000000000001</v>
       </c>
       <c r="E9" s="1">
         <f>0.99</f>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f>3.877</f>
+        <v>3.8769999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -500,15 +535,19 @@
         <f>D10-D$9</f>
         <v>0.38700000000000001</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>3.1</v>
       </c>
       <c r="E10" s="1">
-        <f>$E$9+C10</f>
+        <f>E$9+$C10</f>
         <v>1.377</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1">
+        <f>F$9+$C10</f>
+        <v>4.2639999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -516,15 +555,19 @@
         <f t="shared" ref="C11:C12" si="2">D11-D$9</f>
         <v>0.78699999999999992</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>3.5</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E12" si="3">$E$9+C11</f>
+        <f t="shared" ref="E11:F12" si="3">E$9+$C11</f>
         <v>1.7769999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6639999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -532,12 +575,16 @@
         <f t="shared" si="2"/>
         <v>0.78699999999999992</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>3.5</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="3"/>
         <v>1.7769999999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6639999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>